<commit_message>
creating new branch for chum pc
</commit_message>
<xml_diff>
--- a/experiments/finished exp/young-DSS-exp3/young48_metadata.xlsx
+++ b/experiments/finished exp/young-DSS-exp3/young48_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Chercheurs\Santos_Manuela\Thibault M\gut-microbiota-iron\young-DSS-exp3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Chercheurs\Santos_Manuela\Thibault M\gut-microbiota-iron\experiments\finished exp\young-DSS-exp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276A3F1F-9ED2-4F95-B876-A2843D8C4394}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB8C84E-6FDB-4F61-8F42-7244F41C81DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{9C492067-9821-4BE9-B6E7-34BD5D4FA8D1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>cage</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>oldcage</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>dss</t>
   </si>
 </sst>
 </file>
@@ -637,15 +646,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9407D7-B4D7-455E-A81E-427EC7C4A211}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -656,13 +665,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -672,14 +684,17 @@
       <c r="C2" s="4">
         <v>10971</v>
       </c>
-      <c r="D2" s="1">
-        <v>50</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="D2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1">
+        <v>50</v>
+      </c>
+      <c r="F2" s="5">
         <v>45370</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -687,14 +702,17 @@
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8">
-        <v>50</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="8">
+        <v>50</v>
+      </c>
+      <c r="F3" s="9">
         <v>45372</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -704,14 +722,17 @@
       <c r="C4" s="4">
         <v>995</v>
       </c>
-      <c r="D4" s="1">
-        <v>50</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="D4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="1">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5">
         <v>45372</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -719,14 +740,17 @@
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8">
-        <v>50</v>
-      </c>
-      <c r="E5" s="9">
+      <c r="D5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="8">
+        <v>50</v>
+      </c>
+      <c r="F5" s="9">
         <v>45373</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -736,14 +760,17 @@
       <c r="C6" s="4">
         <v>106</v>
       </c>
-      <c r="D6" s="1">
-        <v>50</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="D6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1">
+        <v>50</v>
+      </c>
+      <c r="F6" s="5">
         <v>45372</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -751,14 +778,17 @@
       <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="8">
-        <v>50</v>
-      </c>
-      <c r="E7" s="9">
+      <c r="D7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="8">
+        <v>50</v>
+      </c>
+      <c r="F7" s="9">
         <v>45370</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -768,14 +798,17 @@
       <c r="C8" s="4">
         <v>108</v>
       </c>
-      <c r="D8" s="1">
-        <v>50</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="D8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1">
+        <v>50</v>
+      </c>
+      <c r="F8" s="5">
         <v>45372</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -783,14 +816,17 @@
       <c r="C9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8">
-        <v>50</v>
-      </c>
-      <c r="E9" s="9">
+      <c r="D9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="8">
+        <v>50</v>
+      </c>
+      <c r="F9" s="9">
         <v>45371</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -800,14 +836,17 @@
       <c r="C10" s="4">
         <v>10968</v>
       </c>
-      <c r="D10" s="1">
-        <v>50</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="D10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="1">
+        <v>50</v>
+      </c>
+      <c r="F10" s="5">
         <v>45370</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -815,14 +854,17 @@
       <c r="C11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="11">
-        <v>50</v>
-      </c>
-      <c r="E11" s="12">
+      <c r="D11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="11">
+        <v>50</v>
+      </c>
+      <c r="F11" s="12">
         <v>45373</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -832,14 +874,17 @@
       <c r="C12" s="13">
         <v>111</v>
       </c>
-      <c r="D12" s="14">
-        <v>50</v>
-      </c>
-      <c r="E12" s="15">
+      <c r="D12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="14">
+        <v>50</v>
+      </c>
+      <c r="F12" s="15">
         <v>45373</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -847,14 +892,17 @@
       <c r="C13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="17">
-        <v>50</v>
-      </c>
-      <c r="E13" s="18">
+      <c r="D13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="17">
+        <v>50</v>
+      </c>
+      <c r="F13" s="18">
         <v>45370</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -864,14 +912,17 @@
       <c r="C14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="11">
-        <v>50</v>
-      </c>
-      <c r="E14" s="12">
+      <c r="D14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="11">
+        <v>50</v>
+      </c>
+      <c r="F14" s="12">
         <v>45372</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -879,14 +930,17 @@
       <c r="C15" s="7">
         <v>10959</v>
       </c>
-      <c r="D15" s="8">
-        <v>50</v>
-      </c>
-      <c r="E15" s="9">
+      <c r="D15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="8">
+        <v>50</v>
+      </c>
+      <c r="F15" s="9">
         <v>45370</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -896,14 +950,17 @@
       <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="1">
-        <v>50</v>
-      </c>
-      <c r="E16" s="5">
+      <c r="D16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="1">
+        <v>50</v>
+      </c>
+      <c r="F16" s="5">
         <v>45372</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -911,14 +968,17 @@
       <c r="C17" s="7">
         <v>10990</v>
       </c>
-      <c r="D17" s="8">
-        <v>50</v>
-      </c>
-      <c r="E17" s="9">
+      <c r="D17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="8">
+        <v>50</v>
+      </c>
+      <c r="F17" s="9">
         <v>45371</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -928,14 +988,17 @@
       <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="1">
-        <v>50</v>
-      </c>
-      <c r="E18" s="5">
+      <c r="D18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="1">
+        <v>50</v>
+      </c>
+      <c r="F18" s="5">
         <v>45373</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8</v>
       </c>
@@ -943,14 +1006,17 @@
       <c r="C19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="11">
-        <v>50</v>
-      </c>
-      <c r="E19" s="12">
+      <c r="D19" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="11">
+        <v>50</v>
+      </c>
+      <c r="F19" s="12">
         <v>45371</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -960,14 +1026,17 @@
       <c r="C20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="14">
-        <v>50</v>
-      </c>
-      <c r="E20" s="15">
+      <c r="D20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="14">
+        <v>50</v>
+      </c>
+      <c r="F20" s="15">
         <v>45373</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -975,14 +1044,17 @@
       <c r="C21" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="17">
-        <v>50</v>
-      </c>
-      <c r="E21" s="18">
+      <c r="D21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="17">
+        <v>50</v>
+      </c>
+      <c r="F21" s="18">
         <v>45372</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -992,14 +1064,17 @@
       <c r="C22" s="10">
         <v>110</v>
       </c>
-      <c r="D22" s="11">
-        <v>50</v>
-      </c>
-      <c r="E22" s="12">
+      <c r="D22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="11">
+        <v>50</v>
+      </c>
+      <c r="F22" s="12">
         <v>45372</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1007,14 +1082,17 @@
       <c r="C23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="8">
-        <v>50</v>
-      </c>
-      <c r="E23" s="9">
+      <c r="D23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="8">
+        <v>50</v>
+      </c>
+      <c r="F23" s="9">
         <v>45371</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1024,14 +1102,17 @@
       <c r="C24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="1">
-        <v>50</v>
-      </c>
-      <c r="E24" s="5">
+      <c r="D24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="1">
+        <v>50</v>
+      </c>
+      <c r="F24" s="5">
         <v>45370</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1039,14 +1120,17 @@
       <c r="C25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="8">
-        <v>50</v>
-      </c>
-      <c r="E25" s="9">
+      <c r="D25" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="8">
+        <v>50</v>
+      </c>
+      <c r="F25" s="9">
         <v>45371</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1056,20 +1140,22 @@
       <c r="C26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="1">
-        <v>50</v>
-      </c>
-      <c r="E26" s="5">
+      <c r="D26" s="4"/>
+      <c r="E26" s="1">
+        <v>50</v>
+      </c>
+      <c r="F26" s="5">
         <v>45370</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="C27" s="19"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="20"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="19"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="20"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1079,14 +1165,17 @@
       <c r="C28" s="4">
         <v>998</v>
       </c>
-      <c r="D28" s="1">
-        <v>500</v>
-      </c>
-      <c r="E28" s="5">
+      <c r="D28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="1">
+        <v>500</v>
+      </c>
+      <c r="F28" s="5">
         <v>45372</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>11</v>
       </c>
@@ -1094,14 +1183,17 @@
       <c r="C29" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="8">
-        <v>500</v>
-      </c>
-      <c r="E29" s="9">
+      <c r="D29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="8">
+        <v>500</v>
+      </c>
+      <c r="F29" s="9">
         <v>45374</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1111,14 +1203,17 @@
       <c r="C30" s="4">
         <v>103</v>
       </c>
-      <c r="D30" s="1">
-        <v>500</v>
-      </c>
-      <c r="E30" s="5">
+      <c r="D30" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="1">
+        <v>500</v>
+      </c>
+      <c r="F30" s="5">
         <v>45372</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>12</v>
       </c>
@@ -1126,14 +1221,17 @@
       <c r="C31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="8">
-        <v>500</v>
-      </c>
-      <c r="E31" s="9">
+      <c r="D31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="8">
+        <v>500</v>
+      </c>
+      <c r="F31" s="9">
         <v>45370</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>
@@ -1143,14 +1241,17 @@
       <c r="C32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="1">
-        <v>500</v>
-      </c>
-      <c r="E32" s="5">
+      <c r="D32" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="1">
+        <v>500</v>
+      </c>
+      <c r="F32" s="5">
         <v>45372</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>13</v>
       </c>
@@ -1158,14 +1259,17 @@
       <c r="C33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="8">
-        <v>500</v>
-      </c>
-      <c r="E33" s="9">
+      <c r="D33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="8">
+        <v>500</v>
+      </c>
+      <c r="F33" s="9">
         <v>45370</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>11</v>
       </c>
@@ -1175,14 +1279,17 @@
       <c r="C34" s="4">
         <v>116</v>
       </c>
-      <c r="D34" s="1">
-        <v>500</v>
-      </c>
-      <c r="E34" s="5">
+      <c r="D34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="1">
+        <v>500</v>
+      </c>
+      <c r="F34" s="5">
         <v>45374</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>12</v>
       </c>
@@ -1190,14 +1297,17 @@
       <c r="C35" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="8">
-        <v>500</v>
-      </c>
-      <c r="E35" s="9">
+      <c r="D35" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="8">
+        <v>500</v>
+      </c>
+      <c r="F35" s="9">
         <v>45370</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>11</v>
       </c>
@@ -1207,14 +1317,17 @@
       <c r="C36" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="1">
-        <v>500</v>
-      </c>
-      <c r="E36" s="5">
+      <c r="D36" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="1">
+        <v>500</v>
+      </c>
+      <c r="F36" s="5">
         <v>45374</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>14</v>
       </c>
@@ -1222,14 +1335,17 @@
       <c r="C37" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="8">
-        <v>500</v>
-      </c>
-      <c r="E37" s="9">
+      <c r="D37" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="8">
+        <v>500</v>
+      </c>
+      <c r="F37" s="9">
         <v>45371</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9</v>
       </c>
@@ -1239,14 +1355,17 @@
       <c r="C38" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="1">
-        <v>500</v>
-      </c>
-      <c r="E38" s="5">
+      <c r="D38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="1">
+        <v>500</v>
+      </c>
+      <c r="F38" s="5">
         <v>45372</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>12</v>
       </c>
@@ -1254,14 +1373,17 @@
       <c r="C39" s="7">
         <v>10955</v>
       </c>
-      <c r="D39" s="8">
-        <v>500</v>
-      </c>
-      <c r="E39" s="9">
+      <c r="D39" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="8">
+        <v>500</v>
+      </c>
+      <c r="F39" s="9">
         <v>45370</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9</v>
       </c>
@@ -1271,14 +1393,17 @@
       <c r="C40" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="1">
-        <v>500</v>
-      </c>
-      <c r="E40" s="5">
+      <c r="D40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="1">
+        <v>500</v>
+      </c>
+      <c r="F40" s="5">
         <v>45372</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>14</v>
       </c>
@@ -1286,14 +1411,17 @@
       <c r="C41" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="8">
-        <v>500</v>
-      </c>
-      <c r="E41" s="9">
+      <c r="D41" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="8">
+        <v>500</v>
+      </c>
+      <c r="F41" s="9">
         <v>45371</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9</v>
       </c>
@@ -1303,14 +1431,17 @@
       <c r="C42" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="1">
-        <v>500</v>
-      </c>
-      <c r="E42" s="5">
+      <c r="D42" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="1">
+        <v>500</v>
+      </c>
+      <c r="F42" s="5">
         <v>45372</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>12</v>
       </c>
@@ -1318,14 +1449,17 @@
       <c r="C43" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="8">
-        <v>500</v>
-      </c>
-      <c r="E43" s="9">
+      <c r="D43" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="8">
+        <v>500</v>
+      </c>
+      <c r="F43" s="9">
         <v>45370</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>13</v>
       </c>
@@ -1335,14 +1469,17 @@
       <c r="C44" s="4">
         <v>10964</v>
       </c>
-      <c r="D44" s="1">
-        <v>500</v>
-      </c>
-      <c r="E44" s="5">
+      <c r="D44" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="1">
+        <v>500</v>
+      </c>
+      <c r="F44" s="5">
         <v>45370</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>14</v>
       </c>
@@ -1350,14 +1487,17 @@
       <c r="C45" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="11">
-        <v>500</v>
-      </c>
-      <c r="E45" s="12">
+      <c r="D45" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="11">
+        <v>500</v>
+      </c>
+      <c r="F45" s="12">
         <v>45371</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>14</v>
       </c>
@@ -1367,14 +1507,17 @@
       <c r="C46" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="1">
-        <v>500</v>
-      </c>
-      <c r="E46" s="5">
+      <c r="D46" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="1">
+        <v>500</v>
+      </c>
+      <c r="F46" s="5">
         <v>45371</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>13</v>
       </c>
@@ -1382,14 +1525,17 @@
       <c r="C47" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D47" s="8">
-        <v>500</v>
-      </c>
-      <c r="E47" s="9">
+      <c r="D47" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" s="8">
+        <v>500</v>
+      </c>
+      <c r="F47" s="9">
         <v>45370</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>13</v>
       </c>
@@ -1399,14 +1545,17 @@
       <c r="C48" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D48" s="1">
-        <v>500</v>
-      </c>
-      <c r="E48" s="5">
+      <c r="D48" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="1">
+        <v>500</v>
+      </c>
+      <c r="F48" s="5">
         <v>45370</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>10</v>
       </c>
@@ -1414,14 +1563,17 @@
       <c r="C49" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="8">
-        <v>500</v>
-      </c>
-      <c r="E49" s="9">
+      <c r="D49" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="8">
+        <v>500</v>
+      </c>
+      <c r="F49" s="9">
         <v>45372</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>15</v>
       </c>
@@ -1431,14 +1583,17 @@
       <c r="C50" s="4">
         <v>10946</v>
       </c>
-      <c r="D50" s="1">
-        <v>500</v>
-      </c>
-      <c r="E50" s="5">
+      <c r="D50" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" s="1">
+        <v>500</v>
+      </c>
+      <c r="F50" s="5">
         <v>45370</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>10</v>
       </c>
@@ -1446,14 +1601,17 @@
       <c r="C51" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="11">
-        <v>500</v>
-      </c>
-      <c r="E51" s="12">
+      <c r="D51" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" s="11">
+        <v>500</v>
+      </c>
+      <c r="F51" s="12">
         <v>45372</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>15</v>
       </c>
@@ -1463,14 +1621,17 @@
       <c r="C52" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D52" s="14">
-        <v>500</v>
-      </c>
-      <c r="E52" s="15">
+      <c r="D52" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="14">
+        <v>500</v>
+      </c>
+      <c r="F52" s="15">
         <v>45370</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>14</v>
       </c>
@@ -1478,10 +1639,13 @@
       <c r="C53" s="16">
         <v>10975</v>
       </c>
-      <c r="D53" s="17">
-        <v>500</v>
-      </c>
-      <c r="E53" s="18">
+      <c r="D53" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" s="17">
+        <v>500</v>
+      </c>
+      <c r="F53" s="18">
         <v>45371</v>
       </c>
     </row>

</xml_diff>